<commit_message>
Add image metadata for OneNet/SOCL-*
Signed-off-by: Richard Marston <rmarston@eonerc.rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/excel-use-cases/OneNet/EACL-PL-04/EACL-PL-04 Introducing BSP.xlsx
+++ b/excel-use-cases/OneNet/EACL-PL-04/EACL-PL-04 Introducing BSP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="241">
   <si>
     <t xml:space="preserve">1 Description of the use case</t>
   </si>
@@ -256,6 +256,9 @@
     <t xml:space="preserve">EACL-PL-04 BSP on Platform_Use case diagram.png</t>
   </si>
   <si>
+    <t xml:space="preserve">EACL-PL-04 BSP on Platform_BUC overview.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 Technical details</t>
   </si>
   <si>
@@ -794,7 +797,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -856,12 +859,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <strike val="true"/>
@@ -1018,7 +1015,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1103,23 +1100,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1211,15 +1200,15 @@
   <dimension ref="A1:CF81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D40" activeCellId="0" sqref="D40"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="86.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="48.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="8" style="0" width="49.18"/>
@@ -1622,25 +1611,25 @@
       <c r="B41" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="22" t="s">
-        <v>56</v>
+      <c r="D41" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1650,7 +1639,7 @@
     <row r="44" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="11"/>
@@ -1660,7 +1649,7 @@
     <row r="45" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="11"/>
@@ -1670,72 +1659,72 @@
     <row r="46" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="52" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="24"/>
+      <c r="B49" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="22"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -1743,7 +1732,7 @@
     <row r="50" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -1752,10 +1741,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="24"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -1763,7 +1752,7 @@
     <row r="52" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="11"/>
@@ -1773,7 +1762,7 @@
     <row r="53" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="11"/>
@@ -1783,7 +1772,7 @@
     <row r="54" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="11"/>
@@ -1793,7 +1782,7 @@
     <row r="55" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
       <c r="B55" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="11"/>
@@ -1803,7 +1792,7 @@
     <row r="56" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="11"/>
@@ -1813,7 +1802,7 @@
     <row r="57" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
       <c r="B57" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="11"/>
@@ -1823,7 +1812,7 @@
     <row r="58" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="11"/>
@@ -1837,17 +1826,17 @@
     </row>
     <row r="60" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1860,7 +1849,7 @@
     <row r="62" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C62" s="8" t="n">
         <v>1</v>
@@ -1887,34 +1876,34 @@
     <row r="63" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
       <c r="B63" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="11"/>
@@ -1927,227 +1916,227 @@
     <row r="65" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
       <c r="B65" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E65" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F65" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F65" s="11" t="s">
-        <v>104</v>
-      </c>
       <c r="G65" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
       <c r="B67" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
       <c r="B68" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
-      <c r="I69" s="27"/>
+        <v>130</v>
+      </c>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25"/>
+      <c r="I69" s="25"/>
     </row>
     <row r="70" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I70" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="N70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="P70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="R70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="T70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="U70" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Y70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AA70" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AB70" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AC70" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AD70" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AE70" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AF70" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AG70" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AH70" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AI70" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AJ70" s="16"/>
       <c r="AK70" s="16"/>
@@ -2202,7 +2191,7 @@
     <row r="71" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
       <c r="B71" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C71" s="16" t="n">
         <v>1.1</v>
@@ -2356,7 +2345,7 @@
     <row r="72" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
       <c r="B72" s="10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="11"/>
@@ -2376,7 +2365,7 @@
       <c r="R72" s="11"/>
       <c r="S72" s="11"/>
       <c r="T72" s="11" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="U72" s="11"/>
       <c r="V72" s="11"/>
@@ -2384,17 +2373,17 @@
       <c r="X72" s="11"/>
       <c r="Y72" s="11"/>
       <c r="Z72" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA72" s="11"/>
       <c r="AB72" s="11"/>
       <c r="AC72" s="11"/>
       <c r="AD72" s="11"/>
       <c r="AE72" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AF72" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AG72" s="11"/>
       <c r="AH72" s="11"/>
@@ -2452,106 +2441,106 @@
     <row r="73" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
       <c r="B73" s="10" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H73" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="L73" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="M73" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="I73" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="J73" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="K73" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="L73" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="M73" s="11" t="s">
-        <v>145</v>
-      </c>
       <c r="N73" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="P73" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="Q73" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="R73" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S73" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="T73" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="U73" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="V73" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="W73" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="S73" s="11" t="s">
+      <c r="X73" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y73" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="T73" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="U73" s="11" t="s">
+      <c r="Z73" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="V73" s="11" t="s">
+      <c r="AA73" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="W73" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="X73" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y73" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z73" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="AA73" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="AB73" s="11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AC73" s="11" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AD73" s="11" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AE73" s="11" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AF73" s="11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AG73" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AH73" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AI73" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AJ73" s="11"/>
       <c r="AK73" s="11"/>
@@ -2606,106 +2595,106 @@
     <row r="74" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="10" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K74" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M74" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N74" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="O74" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P74" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Q74" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="R74" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="S74" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="T74" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="U74" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="V74" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="W74" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="X74" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y74" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="T74" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="U74" s="11" t="s">
+      <c r="Z74" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="V74" s="11" t="s">
+      <c r="AA74" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="W74" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="X74" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="Y74" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="Z74" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="AA74" s="11" t="s">
-        <v>186</v>
-      </c>
       <c r="AB74" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AC74" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AD74" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AE74" s="11" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AF74" s="11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AG74" s="11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AH74" s="11" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AI74" s="11" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AJ74" s="11"/>
       <c r="AK74" s="11"/>
@@ -2760,95 +2749,95 @@
     <row r="75" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
       <c r="B75" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="H75" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="E75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="F75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="H75" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="I75" s="11"/>
       <c r="J75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="K75" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="K75" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="L75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="M75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="N75" s="11" t="s">
         <v>199</v>
-      </c>
-      <c r="M75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="N75" s="11" t="s">
-        <v>198</v>
       </c>
       <c r="O75" s="11"/>
       <c r="P75" s="11" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="Q75" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="R75" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="R75" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="S75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="T75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="U75" s="11"/>
       <c r="V75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="W75" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="X75" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="X75" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="Y75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="Z75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AA75" s="11"/>
       <c r="AB75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AF75" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="AG75" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="AC75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AD75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AE75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AF75" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="AG75" s="11" t="s">
-        <v>198</v>
-      </c>
       <c r="AH75" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AI75" s="11"/>
       <c r="AJ75" s="11"/>
@@ -2904,106 +2893,106 @@
     <row r="76" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
       <c r="B76" s="10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H76" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="I76" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="J76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K76" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L76" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="I76" s="11" t="s">
+      <c r="M76" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="N76" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="J76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K76" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="L76" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="M76" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="N76" s="11" t="s">
-        <v>203</v>
-      </c>
       <c r="O76" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="P76" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q76" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="R76" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="S76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="T76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="U76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="V76" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="W76" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="S76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="T76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="U76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="V76" s="11" t="s">
+      <c r="X76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y76" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB76" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC76" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="W76" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="X76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y76" s="11" t="s">
+      <c r="AD76" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AE76" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF76" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="AG76" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH76" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI76" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="Z76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AB76" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC76" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="AD76" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE76" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AF76" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="AG76" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH76" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AI76" s="11" t="s">
-        <v>204</v>
       </c>
       <c r="AJ76" s="11"/>
       <c r="AK76" s="11"/>
@@ -3058,95 +3047,95 @@
     <row r="77" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
       <c r="B77" s="10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O77" s="11"/>
       <c r="P77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q77" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="R77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="S77" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="Q77" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="R77" s="11" t="s">
+      <c r="T77" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="S77" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="T77" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="U77" s="11"/>
       <c r="V77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="W77" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="X77" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="W77" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="X77" s="11" t="s">
-        <v>203</v>
-      </c>
       <c r="Y77" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z77" s="11" t="s">
         <v>204</v>
-      </c>
-      <c r="Z77" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="AA77" s="11"/>
       <c r="AB77" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AC77" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AD77" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AE77" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AF77" s="11" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG77" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AH77" s="11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AI77" s="11"/>
       <c r="AJ77" s="11"/>
@@ -3202,95 +3191,95 @@
     <row r="78" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="18"/>
       <c r="B78" s="10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I78" s="11"/>
       <c r="J78" s="11" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K78" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M78" s="11" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N78" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O78" s="11"/>
       <c r="P78" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="Q78" s="11" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="R78" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="T78" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="U78" s="11"/>
       <c r="V78" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="W78" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="X78" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="Y78" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z78" s="11" t="s">
         <v>227</v>
-      </c>
-      <c r="W78" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="X78" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="Y78" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z78" s="11" t="s">
-        <v>226</v>
       </c>
       <c r="AA78" s="11"/>
       <c r="AB78" s="11" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AC78" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AD78" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AE78" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AF78" s="11" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG78" s="11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AH78" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AI78" s="11"/>
       <c r="AJ78" s="11"/>
@@ -3346,7 +3335,7 @@
     <row r="79" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="19"/>
       <c r="B79" s="10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="11"/>
@@ -3508,10 +3497,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="11"/>
@@ -3543,19 +3532,19 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add image metadata for ACCEPT, CROSSBOW, MAESHA, PARITY
Signed-off-by: Richard Marston <rmarston@eonerc.rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/excel-use-cases/OneNet/EACL-PL-04/EACL-PL-04 Introducing BSP.xlsx
+++ b/excel-use-cases/OneNet/EACL-PL-04/EACL-PL-04 Introducing BSP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="253">
   <si>
     <t xml:space="preserve">1 Description of the use case</t>
   </si>
@@ -235,13 +235,31 @@
     <t xml:space="preserve">EACL-PL-04 BSP on Platform_BUC overview</t>
   </si>
   <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 3a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 3b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diagram type</t>
   </si>
   <si>
     <t xml:space="preserve">IEC62559.DrawingClassification.use_case_overview</t>
   </si>
   <si>
-    <t xml:space="preserve">IEC62559.DrawingClassification.business_objects_overview</t>
+    <t xml:space="preserve">IEC62559.DrawingClassification.scenario_overview</t>
   </si>
   <si>
     <t xml:space="preserve">Diagram URI type</t>
@@ -257,6 +275,24 @@
   </si>
   <si>
     <t xml:space="preserve">EACL-PL-04 BSP on Platform_BUC overview.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 3a.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 3b.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACL-PL-04 Scenario 5.png</t>
   </si>
   <si>
     <t xml:space="preserve">3 Technical details</t>
@@ -797,7 +833,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -859,6 +895,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <strike val="true"/>
@@ -1015,7 +1057,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1100,15 +1142,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1199,11 +1245,11 @@
   </sheetPr>
   <dimension ref="A1:CF81"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J39" activeCellId="0" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.63"/>
@@ -1576,60 +1622,124 @@
       <c r="D38" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
+      <c r="E38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="20" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
+        <v>64</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="18"/>
       <c r="B40" s="20" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="19"/>
       <c r="B41" s="20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
+        <v>70</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -1639,7 +1749,7 @@
     <row r="44" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
       <c r="B44" s="10" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="11"/>
@@ -1649,7 +1759,7 @@
     <row r="45" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
       <c r="B45" s="10" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="11"/>
@@ -1659,72 +1769,72 @@
     <row r="46" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
       <c r="B46" s="10" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
       <c r="B47" s="10" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="52" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
       <c r="B48" s="10" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
-      <c r="B49" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="22"/>
+      <c r="B49" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="23"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -1732,7 +1842,7 @@
     <row r="50" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -1741,10 +1851,10 @@
     </row>
     <row r="51" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="24"/>
+      <c r="C51" s="25"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -1752,7 +1862,7 @@
     <row r="52" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
       <c r="B52" s="10" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="11"/>
@@ -1762,7 +1872,7 @@
     <row r="53" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
       <c r="B53" s="10" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="11"/>
@@ -1772,7 +1882,7 @@
     <row r="54" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
       <c r="B54" s="10" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="11"/>
@@ -1782,7 +1892,7 @@
     <row r="55" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
       <c r="B55" s="10" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="11"/>
@@ -1792,7 +1902,7 @@
     <row r="56" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
       <c r="B56" s="10" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="11"/>
@@ -1802,7 +1912,7 @@
     <row r="57" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
       <c r="B57" s="10" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="11"/>
@@ -1812,7 +1922,7 @@
     <row r="58" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="10" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="11"/>
@@ -1826,17 +1936,17 @@
     </row>
     <row r="60" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="6" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1849,7 +1959,7 @@
     <row r="62" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="10" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C62" s="8" t="n">
         <v>1</v>
@@ -1876,34 +1986,34 @@
     <row r="63" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
       <c r="B63" s="10" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
       <c r="B64" s="10" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="C64" s="16"/>
       <c r="D64" s="11"/>
@@ -1916,227 +2026,227 @@
     <row r="65" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
       <c r="B65" s="10" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E65" s="11" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
       <c r="B66" s="10" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
       <c r="B67" s="10" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
       <c r="B68" s="10" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
-      <c r="I69" s="25"/>
+        <v>142</v>
+      </c>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
     </row>
     <row r="70" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
       <c r="B70" s="10" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="H70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="I70" s="16" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="J70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="L70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="M70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="N70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="O70" s="16" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="P70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="Q70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="R70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="S70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="T70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="U70" s="16" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="V70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="W70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="X70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Y70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="Z70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="AA70" s="16" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="AB70" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AC70" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AD70" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AE70" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AF70" s="16" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="AG70" s="16" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="AH70" s="16" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="AI70" s="16" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="AJ70" s="16"/>
       <c r="AK70" s="16"/>
@@ -2191,7 +2301,7 @@
     <row r="71" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
       <c r="B71" s="10" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C71" s="16" t="n">
         <v>1.1</v>
@@ -2345,7 +2455,7 @@
     <row r="72" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
       <c r="B72" s="10" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="11"/>
@@ -2365,7 +2475,7 @@
       <c r="R72" s="11"/>
       <c r="S72" s="11"/>
       <c r="T72" s="11" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="U72" s="11"/>
       <c r="V72" s="11"/>
@@ -2373,17 +2483,17 @@
       <c r="X72" s="11"/>
       <c r="Y72" s="11"/>
       <c r="Z72" s="11" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="AA72" s="11"/>
       <c r="AB72" s="11"/>
       <c r="AC72" s="11"/>
       <c r="AD72" s="11"/>
       <c r="AE72" s="11" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="AF72" s="11" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="AG72" s="11"/>
       <c r="AH72" s="11"/>
@@ -2441,106 +2551,106 @@
     <row r="73" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
       <c r="B73" s="10" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E73" s="11" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F73" s="11" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="J73" s="11" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="K73" s="11" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="L73" s="11" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="M73" s="11" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="N73" s="11" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="O73" s="11" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="P73" s="11" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="Q73" s="11" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="R73" s="11" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="S73" s="11" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="T73" s="11" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="U73" s="11" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="V73" s="11" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="W73" s="11" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="X73" s="11" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="Y73" s="11" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="Z73" s="11" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="AA73" s="11" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="AB73" s="11" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="AC73" s="11" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
       <c r="AD73" s="11" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="AE73" s="11" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="AF73" s="11" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="AG73" s="11" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="AH73" s="11" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="AI73" s="11" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="AJ73" s="11"/>
       <c r="AK73" s="11"/>
@@ -2595,106 +2705,106 @@
     <row r="74" customFormat="false" ht="40" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
       <c r="B74" s="10" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="E74" s="11" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="J74" s="11" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="K74" s="11" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="L74" s="11" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="M74" s="11" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="N74" s="11" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="O74" s="11" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="P74" s="11" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="Q74" s="11" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="R74" s="11" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="S74" s="11" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="T74" s="11" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="U74" s="11" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="V74" s="11" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="W74" s="11" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="X74" s="11" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="Y74" s="11" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="Z74" s="11" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="AA74" s="11" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="AB74" s="11" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="AC74" s="11" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="AD74" s="11" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="AE74" s="11" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="AF74" s="11" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="AG74" s="11" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="AH74" s="11" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="AI74" s="11" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="AJ74" s="11"/>
       <c r="AK74" s="11"/>
@@ -2749,95 +2859,95 @@
     <row r="75" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
       <c r="B75" s="10" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="E75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="I75" s="11"/>
       <c r="J75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="K75" s="11" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="L75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="M75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="N75" s="11" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="O75" s="11"/>
       <c r="P75" s="11" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="Q75" s="11" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="R75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="S75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="T75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="U75" s="11"/>
       <c r="V75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="W75" s="11" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="X75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="Y75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="Z75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AA75" s="11"/>
       <c r="AB75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AC75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AD75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AE75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AF75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AG75" s="11" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="AH75" s="11" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="AI75" s="11"/>
       <c r="AJ75" s="11"/>
@@ -2893,106 +3003,106 @@
     <row r="76" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
       <c r="B76" s="10" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E76" s="11" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="I76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="J76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="K76" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="L76" s="11" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="M76" s="11" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="N76" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="O76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="P76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="Q76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="R76" s="11" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="S76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="T76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="U76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="V76" s="11" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="W76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="X76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="Y76" s="11" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="Z76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="AA76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="AB76" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="AC76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="AD76" s="11" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="AE76" s="11" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="AF76" s="11" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="AG76" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="AH76" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="AI76" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="AJ76" s="11"/>
       <c r="AK76" s="11"/>
@@ -3047,95 +3157,95 @@
     <row r="77" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
       <c r="B77" s="10" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="F77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="11" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="K77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="L77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="M77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="O77" s="11"/>
       <c r="P77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="Q77" s="11" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="R77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="S77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="T77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="U77" s="11"/>
       <c r="V77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="W77" s="11" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="X77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="Y77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="Z77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="AA77" s="11"/>
       <c r="AB77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="AC77" s="11" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="AD77" s="11" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="AE77" s="11" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="AF77" s="11" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="AG77" s="11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="AH77" s="11" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="AI77" s="11"/>
       <c r="AJ77" s="11"/>
@@ -3191,95 +3301,95 @@
     <row r="78" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="18"/>
       <c r="B78" s="10" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="H78" s="11" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="I78" s="11"/>
       <c r="J78" s="11" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="K78" s="11" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="L78" s="11" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="M78" s="11" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="N78" s="11" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="O78" s="11"/>
       <c r="P78" s="11" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="Q78" s="11" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="R78" s="11" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="S78" s="11" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="T78" s="11" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="U78" s="11"/>
       <c r="V78" s="11" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="W78" s="11" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="X78" s="11" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="Y78" s="11" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="Z78" s="11" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="AA78" s="11"/>
       <c r="AB78" s="11" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="AC78" s="11" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="AD78" s="11" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="AE78" s="11" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="AF78" s="11" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="AG78" s="11" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="AH78" s="11" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="AI78" s="11"/>
       <c r="AJ78" s="11"/>
@@ -3335,7 +3445,7 @@
     <row r="79" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="19"/>
       <c r="B79" s="10" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="11"/>
@@ -3497,10 +3607,10 @@
     </row>
     <row r="81" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="C81" s="8"/>
       <c r="D81" s="11"/>
@@ -3532,19 +3642,19 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="81.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>